<commit_message>
add hotel base logic
</commit_message>
<xml_diff>
--- a/Document/体系结构设计/DataBaseDraft_v1.xlsx
+++ b/Document/体系结构设计/DataBaseDraft_v1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="20415" windowHeight="8010"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="20412" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Hotel" sheetId="1" r:id="rId1"/>
@@ -331,19 +331,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>北京大酒店</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>302,20161002,20161003;303,20161001,20161024;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京大酒店,西安大酒店,</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -426,11 +426,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -504,6 +509,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -538,6 +544,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -713,26 +720,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="13.875" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="14.875" customWidth="1"/>
-    <col min="8" max="8" width="29.25" customWidth="1"/>
-    <col min="9" max="9" width="34.25" customWidth="1"/>
-    <col min="10" max="10" width="15.625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="29.21875" customWidth="1"/>
+    <col min="9" max="9" width="34.21875" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -764,7 +771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>67</v>
       </c>
@@ -790,13 +797,13 @@
         <v>82</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -815,19 +822,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -838,7 +845,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
@@ -856,31 +863,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
-    <col min="4" max="4" width="15.25" customWidth="1"/>
-    <col min="5" max="6" width="20.25" customWidth="1"/>
-    <col min="7" max="7" width="19.625" customWidth="1"/>
-    <col min="8" max="8" width="11.75" customWidth="1"/>
-    <col min="9" max="9" width="40.75" customWidth="1"/>
-    <col min="10" max="10" width="28.375" customWidth="1"/>
-    <col min="11" max="11" width="13.875" customWidth="1"/>
-    <col min="12" max="12" width="11.625" customWidth="1"/>
-    <col min="14" max="14" width="13.375" customWidth="1"/>
-    <col min="15" max="15" width="12.5" customWidth="1"/>
-    <col min="16" max="16" width="16.25" customWidth="1"/>
+    <col min="1" max="2" width="20.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="6" width="20.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="9" max="9" width="40.77734375" customWidth="1"/>
+    <col min="10" max="10" width="28.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" customWidth="1"/>
+    <col min="16" max="16" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -930,7 +937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>74</v>
       </c>
@@ -988,28 +995,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.25" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
-    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.875" customWidth="1"/>
-    <col min="5" max="5" width="14.25" customWidth="1"/>
-    <col min="6" max="6" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="11.875" customWidth="1"/>
-    <col min="9" max="9" width="15.375" customWidth="1"/>
-    <col min="11" max="11" width="15.125" customWidth="1"/>
-    <col min="12" max="12" width="36.375" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" customWidth="1"/>
+    <col min="12" max="12" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1047,7 +1054,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>73</v>
       </c>
@@ -1092,24 +1099,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
-    <col min="6" max="6" width="12.875" customWidth="1"/>
-    <col min="7" max="7" width="13.25" customWidth="1"/>
-    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -1135,7 +1142,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>66</v>
       </c>
@@ -1168,19 +1175,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1188,7 +1195,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1196,7 +1203,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1204,7 +1211,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1220,7 +1227,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1235,23 +1242,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1268,7 +1275,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>35796</v>
       </c>
@@ -1293,21 +1300,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.125" customWidth="1"/>
-    <col min="3" max="3" width="20.75" customWidth="1"/>
-    <col min="5" max="5" width="50.875" customWidth="1"/>
+    <col min="2" max="2" width="45.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="50.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1324,7 +1331,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1348,21 +1355,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -1374,24 +1381,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>

</xml_diff>